<commit_message>
cierre 25 ago 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  VERDURAS   JULIO     2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #07  J U L I O  2023/BALANCE  VERDURAS   JULIO     2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="11730" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="11730" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="     M A R Z O     2 0 2 3     " sheetId="1" r:id="rId1"/>
@@ -2474,60 +2474,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2590,6 +2536,60 @@
     </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5110,31 +5110,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="257"/>
-      <c r="C1" s="259" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="271" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
     </row>
     <row r="2" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="258"/>
+      <c r="B2" s="270"/>
       <c r="C2" s="4"/>
-      <c r="F2" s="256" t="s">
+      <c r="F2" s="286" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="256"/>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
+      <c r="G2" s="286"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
       <c r="K2" s="176" t="s">
         <v>29</v>
       </c>
@@ -5143,21 +5143,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="262"/>
+      <c r="B3" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="274"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="275" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="263"/>
+      <c r="I3" s="275"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="248" t="s">
+      <c r="R3" s="278" t="s">
         <v>22</v>
       </c>
     </row>
@@ -5170,14 +5170,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="170"/>
-      <c r="E4" s="250" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="251"/>
-      <c r="H4" s="252" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="253"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -5187,11 +5187,11 @@
       <c r="N4" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="254" t="s">
+      <c r="P4" s="284" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="255"/>
-      <c r="R4" s="249"/>
+      <c r="Q4" s="285"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7021,11 +7021,11 @@
       <c r="J45" s="72"/>
       <c r="K45" s="99"/>
       <c r="L45" s="74"/>
-      <c r="M45" s="264">
+      <c r="M45" s="276">
         <f>SUM(M5:M39)</f>
         <v>64841</v>
       </c>
-      <c r="N45" s="273">
+      <c r="N45" s="255">
         <f>SUM(N5:N39)</f>
         <v>0</v>
       </c>
@@ -7057,8 +7057,8 @@
       <c r="J46" s="72"/>
       <c r="K46" s="104"/>
       <c r="L46" s="74"/>
-      <c r="M46" s="265"/>
-      <c r="N46" s="274"/>
+      <c r="M46" s="277"/>
+      <c r="N46" s="256"/>
       <c r="P46" s="96"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -7150,29 +7150,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="275" t="s">
+      <c r="H51" s="257" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="276"/>
+      <c r="I51" s="258"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="277">
+      <c r="K51" s="259">
         <f>I49+L49</f>
         <v>5219.28</v>
       </c>
-      <c r="L51" s="278"/>
-      <c r="M51" s="279">
+      <c r="L51" s="260"/>
+      <c r="M51" s="261">
         <f>N45+M45</f>
         <v>64841</v>
       </c>
-      <c r="N51" s="280"/>
+      <c r="N51" s="262"/>
       <c r="P51" s="96"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D52" s="286" t="s">
+      <c r="D52" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="E52" s="286"/>
+      <c r="E52" s="268"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>46856.369999999995</v>
@@ -7183,20 +7183,20 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D53" s="281"/>
-      <c r="E53" s="281"/>
+      <c r="D53" s="263"/>
+      <c r="E53" s="263"/>
       <c r="F53" s="131">
         <v>0</v>
       </c>
-      <c r="I53" s="282" t="s">
+      <c r="I53" s="264" t="s">
         <v>13</v>
       </c>
-      <c r="J53" s="283"/>
-      <c r="K53" s="284">
+      <c r="J53" s="265"/>
+      <c r="K53" s="266">
         <f>F55+F56+F57</f>
         <v>46856.369999999995</v>
       </c>
-      <c r="L53" s="285"/>
+      <c r="L53" s="267"/>
       <c r="P53" s="96"/>
       <c r="Q53" s="9"/>
     </row>
@@ -7227,11 +7227,11 @@
         <v>15</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="266">
+      <c r="K55" s="248">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L55" s="267"/>
+      <c r="L55" s="249"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -7244,22 +7244,22 @@
     </row>
     <row r="57" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C57" s="150"/>
-      <c r="D57" s="268" t="s">
+      <c r="D57" s="250" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="269"/>
+      <c r="E57" s="251"/>
       <c r="F57" s="151">
         <v>0</v>
       </c>
-      <c r="I57" s="270" t="s">
+      <c r="I57" s="252" t="s">
         <v>18</v>
       </c>
-      <c r="J57" s="271"/>
-      <c r="K57" s="272">
+      <c r="J57" s="253"/>
+      <c r="K57" s="254">
         <f>K53+K55</f>
         <v>46856.369999999995</v>
       </c>
-      <c r="L57" s="272"/>
+      <c r="L57" s="254"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -7384,6 +7384,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="I57:J57"/>
@@ -7396,16 +7406,6 @@
     <mergeCell ref="I53:J53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="D52:E52"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7451,31 +7451,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="257"/>
-      <c r="C1" s="259" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="271" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
     </row>
     <row r="2" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="258"/>
+      <c r="B2" s="270"/>
       <c r="C2" s="4"/>
-      <c r="F2" s="256" t="s">
+      <c r="F2" s="286" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="256"/>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
+      <c r="G2" s="286"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
       <c r="K2" s="197" t="s">
         <v>29</v>
       </c>
@@ -7486,21 +7486,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="262"/>
+      <c r="B3" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="274"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="275" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="263"/>
+      <c r="I3" s="275"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="248" t="s">
+      <c r="R3" s="278" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7513,14 +7513,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="170"/>
-      <c r="E4" s="250" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="251"/>
-      <c r="H4" s="252" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="253"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -7530,11 +7530,11 @@
       <c r="N4" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="254" t="s">
+      <c r="P4" s="284" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="255"/>
-      <c r="R4" s="249"/>
+      <c r="Q4" s="285"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -10073,11 +10073,11 @@
       <c r="J63" s="72"/>
       <c r="K63" s="99"/>
       <c r="L63" s="74"/>
-      <c r="M63" s="264">
+      <c r="M63" s="276">
         <f>SUM(M5:M48)</f>
         <v>88632</v>
       </c>
-      <c r="N63" s="273">
+      <c r="N63" s="255">
         <f>SUM(N5:N48)</f>
         <v>46604</v>
       </c>
@@ -10109,8 +10109,8 @@
       <c r="J64" s="72"/>
       <c r="K64" s="104"/>
       <c r="L64" s="74"/>
-      <c r="M64" s="265"/>
-      <c r="N64" s="274"/>
+      <c r="M64" s="277"/>
+      <c r="N64" s="256"/>
       <c r="P64" s="96"/>
       <c r="Q64" s="9"/>
       <c r="R64" s="13">
@@ -10202,29 +10202,29 @@
       <c r="A69" s="133"/>
       <c r="B69" s="134"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="275" t="s">
+      <c r="H69" s="257" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="276"/>
+      <c r="I69" s="258"/>
       <c r="J69" s="135"/>
-      <c r="K69" s="277">
+      <c r="K69" s="259">
         <f>I67+L67</f>
         <v>6435</v>
       </c>
-      <c r="L69" s="278"/>
-      <c r="M69" s="279">
+      <c r="L69" s="260"/>
+      <c r="M69" s="261">
         <f>N63+M63</f>
         <v>135236</v>
       </c>
-      <c r="N69" s="280"/>
+      <c r="N69" s="262"/>
       <c r="P69" s="96"/>
       <c r="Q69" s="9"/>
     </row>
     <row r="70" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D70" s="286" t="s">
+      <c r="D70" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="286"/>
+      <c r="E70" s="268"/>
       <c r="F70" s="136">
         <f>F67-K69-C67</f>
         <v>65323.966999999975</v>
@@ -10235,20 +10235,20 @@
       <c r="Q70" s="9"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="281"/>
-      <c r="E71" s="281"/>
+      <c r="D71" s="263"/>
+      <c r="E71" s="263"/>
       <c r="F71" s="131">
         <v>0</v>
       </c>
-      <c r="I71" s="282" t="s">
+      <c r="I71" s="264" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="283"/>
-      <c r="K71" s="284">
+      <c r="J71" s="265"/>
+      <c r="K71" s="266">
         <f>F73+F74+F75</f>
         <v>65323.966999999975</v>
       </c>
-      <c r="L71" s="285"/>
+      <c r="L71" s="267"/>
       <c r="P71" s="96"/>
       <c r="Q71" s="9"/>
     </row>
@@ -10279,11 +10279,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="147"/>
-      <c r="K73" s="266">
+      <c r="K73" s="248">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L73" s="267"/>
+      <c r="L73" s="249"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="148" t="s">
@@ -10296,22 +10296,22 @@
     </row>
     <row r="75" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="150"/>
-      <c r="D75" s="268" t="s">
+      <c r="D75" s="250" t="s">
         <v>17</v>
       </c>
-      <c r="E75" s="269"/>
+      <c r="E75" s="251"/>
       <c r="F75" s="151">
         <v>0</v>
       </c>
-      <c r="I75" s="270" t="s">
+      <c r="I75" s="252" t="s">
         <v>18</v>
       </c>
-      <c r="J75" s="271"/>
-      <c r="K75" s="272">
+      <c r="J75" s="253"/>
+      <c r="K75" s="254">
         <f>K71+K73</f>
         <v>65323.966999999975</v>
       </c>
-      <c r="L75" s="272"/>
+      <c r="L75" s="254"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="152"/>
@@ -10436,6 +10436,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -10446,18 +10458,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="M69:N69"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.33" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10500,31 +10500,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="257"/>
-      <c r="C1" s="259" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="271" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
     </row>
     <row r="2" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="258"/>
+      <c r="B2" s="270"/>
       <c r="C2" s="4"/>
-      <c r="F2" s="256" t="s">
+      <c r="F2" s="286" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="256"/>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
+      <c r="G2" s="286"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
       <c r="K2" s="197" t="s">
         <v>29</v>
       </c>
@@ -10535,21 +10535,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="262"/>
+      <c r="B3" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="274"/>
       <c r="D3" s="2"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="275" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="263"/>
+      <c r="I3" s="275"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="248" t="s">
+      <c r="R3" s="278" t="s">
         <v>22</v>
       </c>
     </row>
@@ -10562,14 +10562,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="218"/>
-      <c r="E4" s="250" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="251"/>
-      <c r="H4" s="252" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="253"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -10579,11 +10579,11 @@
       <c r="N4" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="254" t="s">
+      <c r="P4" s="284" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="255"/>
-      <c r="R4" s="249"/>
+      <c r="Q4" s="285"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -12895,11 +12895,11 @@
       <c r="J56" s="72"/>
       <c r="K56" s="99"/>
       <c r="L56" s="74"/>
-      <c r="M56" s="264">
+      <c r="M56" s="276">
         <f>SUM(M5:M48)</f>
         <v>41580</v>
       </c>
-      <c r="N56" s="273">
+      <c r="N56" s="255">
         <f>SUM(N5:N48)</f>
         <v>50201</v>
       </c>
@@ -12931,8 +12931,8 @@
       <c r="J57" s="72"/>
       <c r="K57" s="104"/>
       <c r="L57" s="74"/>
-      <c r="M57" s="265"/>
-      <c r="N57" s="274"/>
+      <c r="M57" s="277"/>
+      <c r="N57" s="256"/>
       <c r="P57" s="96"/>
       <c r="Q57" s="9"/>
       <c r="R57" s="13">
@@ -13006,29 +13006,29 @@
       <c r="A61" s="133"/>
       <c r="B61" s="134"/>
       <c r="C61" s="1"/>
-      <c r="H61" s="275" t="s">
+      <c r="H61" s="257" t="s">
         <v>11</v>
       </c>
-      <c r="I61" s="276"/>
+      <c r="I61" s="258"/>
       <c r="J61" s="135"/>
-      <c r="K61" s="277">
+      <c r="K61" s="259">
         <f>I59+L59</f>
         <v>4723.5599999999995</v>
       </c>
-      <c r="L61" s="278"/>
-      <c r="M61" s="279">
+      <c r="L61" s="260"/>
+      <c r="M61" s="261">
         <f>N56+M56</f>
         <v>91781</v>
       </c>
-      <c r="N61" s="280"/>
+      <c r="N61" s="262"/>
       <c r="P61" s="96"/>
       <c r="Q61" s="9"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D62" s="286" t="s">
+      <c r="D62" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="286"/>
+      <c r="E62" s="268"/>
       <c r="F62" s="136">
         <f>F59-K61-C59</f>
         <v>70157.13</v>
@@ -13039,20 +13039,20 @@
       <c r="Q62" s="9"/>
     </row>
     <row r="63" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D63" s="281"/>
-      <c r="E63" s="281"/>
+      <c r="D63" s="263"/>
+      <c r="E63" s="263"/>
       <c r="F63" s="131">
         <v>0</v>
       </c>
-      <c r="I63" s="282" t="s">
+      <c r="I63" s="264" t="s">
         <v>13</v>
       </c>
-      <c r="J63" s="283"/>
-      <c r="K63" s="284">
+      <c r="J63" s="265"/>
+      <c r="K63" s="266">
         <f>F65+F66+F67</f>
         <v>70157.13</v>
       </c>
-      <c r="L63" s="285"/>
+      <c r="L63" s="267"/>
       <c r="P63" s="96"/>
       <c r="Q63" s="9"/>
     </row>
@@ -13083,11 +13083,11 @@
         <v>15</v>
       </c>
       <c r="J65" s="147"/>
-      <c r="K65" s="266">
+      <c r="K65" s="248">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L65" s="267"/>
+      <c r="L65" s="249"/>
     </row>
     <row r="66" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="221" t="s">
@@ -13100,22 +13100,22 @@
     </row>
     <row r="67" spans="2:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C67" s="150"/>
-      <c r="D67" s="268" t="s">
+      <c r="D67" s="250" t="s">
         <v>17</v>
       </c>
-      <c r="E67" s="269"/>
+      <c r="E67" s="251"/>
       <c r="F67" s="151">
         <v>0</v>
       </c>
-      <c r="I67" s="270" t="s">
+      <c r="I67" s="252" t="s">
         <v>18</v>
       </c>
-      <c r="J67" s="271"/>
-      <c r="K67" s="272">
+      <c r="J67" s="253"/>
+      <c r="K67" s="254">
         <f>K63+K65</f>
         <v>70157.13</v>
       </c>
-      <c r="L67" s="272"/>
+      <c r="L67" s="254"/>
     </row>
     <row r="68" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C68" s="152"/>
@@ -13243,6 +13243,18 @@
     <sortCondition ref="B38:B56"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -13253,18 +13265,6 @@
     <mergeCell ref="H61:I61"/>
     <mergeCell ref="K61:L61"/>
     <mergeCell ref="M61:N61"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:L67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13280,8 +13280,8 @@
   </sheetPr>
   <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" topLeftCell="H37" workbookViewId="0">
+      <selection activeCell="S53" sqref="S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13307,31 +13307,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="257"/>
-      <c r="C1" s="259" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="271" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
     </row>
     <row r="2" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="258"/>
+      <c r="B2" s="270"/>
       <c r="C2" s="4"/>
-      <c r="F2" s="256" t="s">
+      <c r="F2" s="286" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="256"/>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
+      <c r="G2" s="286"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
       <c r="K2" s="197" t="s">
         <v>29</v>
       </c>
@@ -13342,21 +13342,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="262"/>
+      <c r="B3" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="274"/>
       <c r="D3" s="2"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="275" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="263"/>
+      <c r="I3" s="275"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="248" t="s">
+      <c r="R3" s="278" t="s">
         <v>22</v>
       </c>
     </row>
@@ -13369,14 +13369,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="218"/>
-      <c r="E4" s="250" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="251"/>
-      <c r="H4" s="252" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="253"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -13386,11 +13386,11 @@
       <c r="N4" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="254" t="s">
+      <c r="P4" s="284" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="255"/>
-      <c r="R4" s="249"/>
+      <c r="Q4" s="285"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -15707,11 +15707,11 @@
       <c r="J56" s="72"/>
       <c r="K56" s="99"/>
       <c r="L56" s="74"/>
-      <c r="M56" s="264">
+      <c r="M56" s="276">
         <f>SUM(M5:M48)</f>
         <v>32186</v>
       </c>
-      <c r="N56" s="273">
+      <c r="N56" s="255">
         <f>SUM(N5:N48)</f>
         <v>58977</v>
       </c>
@@ -15720,8 +15720,8 @@
         <v>91163</v>
       </c>
       <c r="Q56" s="100">
-        <f t="shared" si="1"/>
-        <v>91163</v>
+        <f>SUM(Q5:Q55)</f>
+        <v>-486</v>
       </c>
       <c r="R56" s="101">
         <f>SUM(R5:R48)</f>
@@ -15743,8 +15743,8 @@
       <c r="J57" s="72"/>
       <c r="K57" s="104"/>
       <c r="L57" s="74"/>
-      <c r="M57" s="265"/>
-      <c r="N57" s="274"/>
+      <c r="M57" s="277"/>
+      <c r="N57" s="256"/>
       <c r="P57" s="96"/>
       <c r="Q57" s="9"/>
       <c r="R57" s="13">
@@ -15818,29 +15818,29 @@
       <c r="A61" s="133"/>
       <c r="B61" s="134"/>
       <c r="C61" s="1"/>
-      <c r="H61" s="275" t="s">
+      <c r="H61" s="257" t="s">
         <v>11</v>
       </c>
-      <c r="I61" s="276"/>
+      <c r="I61" s="258"/>
       <c r="J61" s="135"/>
-      <c r="K61" s="277">
+      <c r="K61" s="259">
         <f>I59+L59</f>
         <v>30105.55</v>
       </c>
-      <c r="L61" s="278"/>
-      <c r="M61" s="279">
+      <c r="L61" s="260"/>
+      <c r="M61" s="261">
         <f>N56+M56</f>
         <v>91163</v>
       </c>
-      <c r="N61" s="280"/>
+      <c r="N61" s="262"/>
       <c r="P61" s="96"/>
       <c r="Q61" s="9"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D62" s="286" t="s">
+      <c r="D62" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="286"/>
+      <c r="E62" s="268"/>
       <c r="F62" s="136">
         <f>F59-K61-C59</f>
         <v>50573.330000000016</v>
@@ -15851,20 +15851,20 @@
       <c r="Q62" s="9"/>
     </row>
     <row r="63" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D63" s="281"/>
-      <c r="E63" s="281"/>
+      <c r="D63" s="263"/>
+      <c r="E63" s="263"/>
       <c r="F63" s="131">
         <v>0</v>
       </c>
-      <c r="I63" s="282" t="s">
+      <c r="I63" s="264" t="s">
         <v>13</v>
       </c>
-      <c r="J63" s="283"/>
-      <c r="K63" s="284">
+      <c r="J63" s="265"/>
+      <c r="K63" s="266">
         <f>F65+F66+F67</f>
         <v>50573.330000000016</v>
       </c>
-      <c r="L63" s="285"/>
+      <c r="L63" s="267"/>
       <c r="P63" s="96"/>
       <c r="Q63" s="9"/>
     </row>
@@ -15895,11 +15895,11 @@
         <v>15</v>
       </c>
       <c r="J65" s="147"/>
-      <c r="K65" s="266">
+      <c r="K65" s="248">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L65" s="267"/>
+      <c r="L65" s="249"/>
     </row>
     <row r="66" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="221" t="s">
@@ -15912,22 +15912,22 @@
     </row>
     <row r="67" spans="2:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C67" s="150"/>
-      <c r="D67" s="268" t="s">
+      <c r="D67" s="250" t="s">
         <v>17</v>
       </c>
-      <c r="E67" s="269"/>
+      <c r="E67" s="251"/>
       <c r="F67" s="151">
         <v>0</v>
       </c>
-      <c r="I67" s="270" t="s">
+      <c r="I67" s="252" t="s">
         <v>18</v>
       </c>
-      <c r="J67" s="271"/>
-      <c r="K67" s="272">
+      <c r="J67" s="253"/>
+      <c r="K67" s="254">
         <f>K63+K65</f>
         <v>50573.330000000016</v>
       </c>
-      <c r="L67" s="272"/>
+      <c r="L67" s="254"/>
     </row>
     <row r="68" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C68" s="152"/>
@@ -16052,6 +16052,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -16062,18 +16074,6 @@
     <mergeCell ref="H61:I61"/>
     <mergeCell ref="K61:L61"/>
     <mergeCell ref="M61:N61"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:L67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16089,7 +16089,7 @@
   </sheetPr>
   <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
@@ -16116,31 +16116,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="257"/>
-      <c r="C1" s="259" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="271" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="260"/>
-      <c r="E1" s="260"/>
-      <c r="F1" s="260"/>
-      <c r="G1" s="260"/>
-      <c r="H1" s="260"/>
-      <c r="I1" s="260"/>
-      <c r="J1" s="260"/>
-      <c r="K1" s="260"/>
-      <c r="L1" s="260"/>
-      <c r="M1" s="260"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
     </row>
     <row r="2" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="258"/>
+      <c r="B2" s="270"/>
       <c r="C2" s="4"/>
-      <c r="F2" s="256" t="s">
+      <c r="F2" s="286" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="256"/>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
+      <c r="G2" s="286"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
       <c r="K2" s="197" t="s">
         <v>29</v>
       </c>
@@ -16151,21 +16151,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="261" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="262"/>
+      <c r="B3" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="274"/>
       <c r="D3" s="2"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="275" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="263"/>
+      <c r="I3" s="275"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="248" t="s">
+      <c r="R3" s="278" t="s">
         <v>22</v>
       </c>
     </row>
@@ -16178,14 +16178,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="218"/>
-      <c r="E4" s="250" t="s">
+      <c r="E4" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="251"/>
-      <c r="H4" s="252" t="s">
+      <c r="F4" s="281"/>
+      <c r="H4" s="282" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="253"/>
+      <c r="I4" s="283"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -16195,11 +16195,11 @@
       <c r="N4" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="254" t="s">
+      <c r="P4" s="284" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="255"/>
-      <c r="R4" s="249"/>
+      <c r="Q4" s="285"/>
+      <c r="R4" s="279"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -16344,7 +16344,7 @@
       <c r="N8" s="31"/>
       <c r="O8" s="241"/>
       <c r="P8" s="33">
-        <f t="shared" ref="P8:Q56" si="1">N8+M8+L8+I8+C8</f>
+        <f t="shared" ref="P8:P56" si="1">N8+M8+L8+I8+C8</f>
         <v>0</v>
       </c>
       <c r="Q8" s="34">
@@ -17915,11 +17915,11 @@
       <c r="J56" s="72"/>
       <c r="K56" s="99"/>
       <c r="L56" s="74"/>
-      <c r="M56" s="264">
+      <c r="M56" s="276">
         <f>SUM(M5:M48)</f>
         <v>0</v>
       </c>
-      <c r="N56" s="273">
+      <c r="N56" s="255">
         <f>SUM(N5:N48)</f>
         <v>0</v>
       </c>
@@ -17951,8 +17951,8 @@
       <c r="J57" s="72"/>
       <c r="K57" s="104"/>
       <c r="L57" s="74"/>
-      <c r="M57" s="265"/>
-      <c r="N57" s="274"/>
+      <c r="M57" s="277"/>
+      <c r="N57" s="256"/>
       <c r="P57" s="96"/>
       <c r="Q57" s="9"/>
       <c r="R57" s="13">
@@ -18026,29 +18026,29 @@
       <c r="A61" s="133"/>
       <c r="B61" s="134"/>
       <c r="C61" s="1"/>
-      <c r="H61" s="275" t="s">
+      <c r="H61" s="257" t="s">
         <v>11</v>
       </c>
-      <c r="I61" s="276"/>
+      <c r="I61" s="258"/>
       <c r="J61" s="135"/>
-      <c r="K61" s="277">
+      <c r="K61" s="259">
         <f>I59+L59</f>
         <v>0</v>
       </c>
-      <c r="L61" s="278"/>
-      <c r="M61" s="279">
+      <c r="L61" s="260"/>
+      <c r="M61" s="261">
         <f>N56+M56</f>
         <v>0</v>
       </c>
-      <c r="N61" s="280"/>
+      <c r="N61" s="262"/>
       <c r="P61" s="96"/>
       <c r="Q61" s="9"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D62" s="286" t="s">
+      <c r="D62" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="E62" s="286"/>
+      <c r="E62" s="268"/>
       <c r="F62" s="136">
         <f>F59-K61-C59</f>
         <v>0</v>
@@ -18059,20 +18059,20 @@
       <c r="Q62" s="9"/>
     </row>
     <row r="63" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D63" s="281"/>
-      <c r="E63" s="281"/>
+      <c r="D63" s="263"/>
+      <c r="E63" s="263"/>
       <c r="F63" s="131">
         <v>0</v>
       </c>
-      <c r="I63" s="282" t="s">
+      <c r="I63" s="264" t="s">
         <v>13</v>
       </c>
-      <c r="J63" s="283"/>
-      <c r="K63" s="284">
+      <c r="J63" s="265"/>
+      <c r="K63" s="266">
         <f>F65+F66+F67</f>
         <v>0</v>
       </c>
-      <c r="L63" s="285"/>
+      <c r="L63" s="267"/>
       <c r="P63" s="96"/>
       <c r="Q63" s="9"/>
     </row>
@@ -18103,11 +18103,11 @@
         <v>15</v>
       </c>
       <c r="J65" s="147"/>
-      <c r="K65" s="266">
+      <c r="K65" s="248">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L65" s="267"/>
+      <c r="L65" s="249"/>
     </row>
     <row r="66" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D66" s="221" t="s">
@@ -18120,22 +18120,22 @@
     </row>
     <row r="67" spans="2:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C67" s="150"/>
-      <c r="D67" s="268" t="s">
+      <c r="D67" s="250" t="s">
         <v>17</v>
       </c>
-      <c r="E67" s="269"/>
+      <c r="E67" s="251"/>
       <c r="F67" s="151">
         <v>0</v>
       </c>
-      <c r="I67" s="270" t="s">
+      <c r="I67" s="252" t="s">
         <v>18</v>
       </c>
-      <c r="J67" s="271"/>
-      <c r="K67" s="272">
+      <c r="J67" s="253"/>
+      <c r="K67" s="254">
         <f>K63+K65</f>
         <v>0</v>
       </c>
-      <c r="L67" s="272"/>
+      <c r="L67" s="254"/>
     </row>
     <row r="68" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C68" s="152"/>
@@ -18260,6 +18260,21 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M56:M57"/>
+    <mergeCell ref="N56:N57"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="M61:N61"/>
     <mergeCell ref="D63:E63"/>
     <mergeCell ref="I63:J63"/>
     <mergeCell ref="K63:L63"/>
@@ -18267,21 +18282,6 @@
     <mergeCell ref="D67:E67"/>
     <mergeCell ref="I67:J67"/>
     <mergeCell ref="K67:L67"/>
-    <mergeCell ref="M56:M57"/>
-    <mergeCell ref="N56:N57"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="M61:N61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>